<commit_message>
Correções no não terminal "Expressao"
</commit_message>
<xml_diff>
--- a/Documentação/Gramática.xlsx
+++ b/Documentação/Gramática.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\GitHub\analisador_sintatico\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ECF33A2A-2CFC-4079-B932-C72DED9ABDA0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3F035D93-CBEC-4659-8D33-83E799A254F4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="21570" windowHeight="7980" xr2:uid="{5EF7EE27-F00D-46A1-9DA9-1812314FC15C}"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="21570" windowHeight="7980" xr2:uid="{5EF7EE27-F00D-46A1-9DA9-1812314FC15C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="144">
   <si>
     <t>Compilador</t>
   </si>
@@ -159,36 +159,6 @@
     <t>"leia" "(" ID ")" ";"</t>
   </si>
   <si>
-    <t>Op</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Ou" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">| "E" </t>
-  </si>
-  <si>
-    <t>| "&lt;="</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> | "&gt;" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">| "&gt;=" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">| "=" </t>
-  </si>
-  <si>
-    <t>| "&lt;&gt;"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">| "*" </t>
-  </si>
-  <si>
-    <t>| "+"</t>
-  </si>
-  <si>
     <t>OpUnario</t>
   </si>
   <si>
@@ -438,6 +408,706 @@
     </r>
   </si>
   <si>
+    <t>fim</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>subrotina</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>retorne</t>
+  </si>
+  <si>
+    <t>logico</t>
+  </si>
+  <si>
+    <t>numerico</t>
+  </si>
+  <si>
+    <t>literal</t>
+  </si>
+  <si>
+    <t>nulo</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>inicio</t>
+  </si>
+  <si>
+    <t>enquanto</t>
+  </si>
+  <si>
+    <t>faca</t>
+  </si>
+  <si>
+    <t>para</t>
+  </si>
+  <si>
+    <t>ate</t>
+  </si>
+  <si>
+    <t>&lt;--</t>
+  </si>
+  <si>
+    <t>escreva</t>
+  </si>
+  <si>
+    <t>leia</t>
+  </si>
+  <si>
+    <t>Ou</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&lt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>/*</t>
+  </si>
+  <si>
+    <t>*/</t>
+  </si>
+  <si>
+    <t>Terminais:</t>
+  </si>
+  <si>
+    <t>ListaParam2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Param</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaParam2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"," </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaParam</t>
+    </r>
+  </si>
+  <si>
+    <t>CmdSe1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"se" "(" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expressao</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ")" "inicio" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaCmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "fim" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CmdSe1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> "senao" "inicio" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaCmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "fim"</t>
+    </r>
+  </si>
+  <si>
+    <t>ListaID1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ID </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaID1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"," </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaID</t>
+    </r>
+  </si>
+  <si>
+    <t>DeclaraVar1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tipo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ";" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DeclaraVar1</t>
+    </r>
+  </si>
+  <si>
+    <t>Declara</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"algoritmo" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Declara</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaCmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "fim" "algoritmo" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaRotina</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"declare" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DeclaraVar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"subrotina" ID "(" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaParam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ")" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Declara</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaCmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Retorno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "fim" "subrotina"</t>
+    </r>
+  </si>
+  <si>
+    <t>ListaRotina1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rotina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaRotina1</t>
+    </r>
+  </si>
+  <si>
+    <t>ListaCmd1</t>
+  </si>
+  <si>
+    <t>Cmd ListaCmd1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListaCmd1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Expressao2</t>
+  </si>
+  <si>
+    <t>Expressao3</t>
+  </si>
+  <si>
+    <t>Expressao4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"," </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expressao Expressao4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> "(" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expressao3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ")"</t>
+    </r>
+  </si>
+  <si>
+    <t>Expressao Expressao4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">| "(" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expressao</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ")" </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">| </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OpUnario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expressao</t>
+    </r>
+  </si>
+  <si>
+    <t>| "falso"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| "verdadeiro" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> | Literal </t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">ID "(" </t>
     </r>
@@ -450,138 +1120,88 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Expressao</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ("," </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)∗ )? ")" ";"</t>
-    </r>
-  </si>
-  <si>
-    <t>fim</t>
-  </si>
-  <si>
-    <t>:</t>
-  </si>
-  <si>
-    <t>subrotina</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>retorne</t>
-  </si>
-  <si>
-    <t>logico</t>
-  </si>
-  <si>
-    <t>numerico</t>
-  </si>
-  <si>
-    <t>literal</t>
-  </si>
-  <si>
-    <t>nulo</t>
-  </si>
-  <si>
-    <t>se</t>
-  </si>
-  <si>
-    <t>inicio</t>
-  </si>
-  <si>
-    <t>enquanto</t>
-  </si>
-  <si>
-    <t>faca</t>
-  </si>
-  <si>
-    <t>para</t>
-  </si>
-  <si>
-    <t>ate</t>
-  </si>
-  <si>
-    <t>&lt;--</t>
-  </si>
-  <si>
-    <t>escreva</t>
-  </si>
-  <si>
-    <t>leia</t>
-  </si>
-  <si>
-    <t>Ou</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>&lt;</t>
-  </si>
-  <si>
-    <t>&lt;&gt;</t>
-  </si>
-  <si>
-    <t>&lt;=</t>
-  </si>
-  <si>
-    <t>&gt;</t>
-  </si>
-  <si>
-    <t>&gt;=</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>//</t>
-  </si>
-  <si>
-    <t>/*</t>
-  </si>
-  <si>
-    <t>*/</t>
-  </si>
-  <si>
-    <t>Terminais:</t>
+      <t>Expressao3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ")" ";"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Numerico</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">|ID </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expressao2</t>
+    </r>
+  </si>
+  <si>
+    <t>ExpressaoRelacional</t>
+  </si>
+  <si>
+    <t>ExpressaoAritmetica2</t>
+  </si>
+  <si>
+    <t>ExpressaoResidual</t>
+  </si>
+  <si>
+    <t>ExpressaoRelacional Expressao'</t>
+  </si>
+  <si>
+    <t>Expressao'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Ou"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExpressaoRelacional Expressao'</t>
+    </r>
   </si>
   <si>
     <r>
@@ -589,21 +1209,57 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Op1</t>
-    </r>
-  </si>
-  <si>
-    <t>Op1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"&lt;" </t>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"E"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExpressaoRelacional Expressao'</t>
+    </r>
+  </si>
+  <si>
+    <t>ExpressaoAritmetica</t>
+  </si>
+  <si>
+    <t>ExpressaoAritmetica ExpressaoRelacional'</t>
+  </si>
+  <si>
+    <t>ExpressaoRelacional'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&lt;"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExpressaoAritmetica ExpressaoRelacional'</t>
+    </r>
   </si>
   <si>
     <r>
@@ -611,18 +1267,25 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Op2</t>
-    </r>
-  </si>
-  <si>
-    <t>Op2</t>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&lt;="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExpressaoAritmetica ExpressaoRelacional'</t>
+    </r>
   </si>
   <si>
     <r>
@@ -630,571 +1293,24 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Op3</t>
-    </r>
-  </si>
-  <si>
-    <t>Op3</t>
-  </si>
-  <si>
-    <t>ListaParam2</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Param</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaParam2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">"," </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaParam</t>
-    </r>
-  </si>
-  <si>
-    <t>CmdSe1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">"se" "(" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ")" "inicio" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaCmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "fim" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CmdSe1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> "senao" "inicio" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaCmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "fim"</t>
-    </r>
-  </si>
-  <si>
-    <t>Expressao1</t>
-  </si>
-  <si>
-    <t>ListaID1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ID </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaID1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">"," </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaID</t>
-    </r>
-  </si>
-  <si>
-    <t>DeclaraVar1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Tipo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ";" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DeclaraVar1</t>
-    </r>
-  </si>
-  <si>
-    <t>Declara</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">"algoritmo" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Declara</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaCmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "fim" "algoritmo" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaRotina</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">"declare" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DeclaraVar</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">"subrotina" ID "(" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaParam</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ")" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Declara</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaCmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Retorno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "fim" "subrotina"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">"/" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"-" </t>
-  </si>
-  <si>
-    <t>ListaRotina1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Rotina</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaRotina1</t>
-    </r>
-  </si>
-  <si>
-    <t>ListaCmd1</t>
-  </si>
-  <si>
-    <t>Cmd ListaCmd1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ListaCmd1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>Expressao2</t>
-  </si>
-  <si>
-    <t>Op Expressao Expressao1</t>
-  </si>
-  <si>
-    <r>
-      <t>| Numerico</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Expressao1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> | Literal </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">| "verdadeiro" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">| "falso" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao1</t>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&gt;"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExpressaoAritmetica ExpressaoRelacional'</t>
     </r>
   </si>
   <si>
@@ -1203,161 +1319,187 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OpUnario</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">| "(" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ")" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ID </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao2 Expressao1</t>
-    </r>
-  </si>
-  <si>
-    <t>Expressao3</t>
-  </si>
-  <si>
-    <t>Expressao4</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">"," </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao Expressao4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> "(" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expressao3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ")"</t>
-    </r>
-  </si>
-  <si>
-    <t>Expressao Expressao4</t>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&gt;="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExpressaoAritmetica ExpressaoRelacional'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">| </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ExpressaoAritmetica ExpressaoRelacional'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">| </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&lt;&gt;"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExpressaoAritmetica ExpressaoRelacional'</t>
+    </r>
+  </si>
+  <si>
+    <t>ExpressaoAritmetica2 ExpressaoAritmetica'</t>
+  </si>
+  <si>
+    <t>ExpressaoAritmetica'</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">| </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"+"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExpressaoAritmetica2 ExpressaoAritmetica'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"-"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ExpressaoAritmetica2 ExpressaoAritmetica'</t>
+    </r>
+  </si>
+  <si>
+    <t>ExpressaoAritmetica2'</t>
+  </si>
+  <si>
+    <t>ExpressaoResidual ExpressaoAritmetica2'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"/"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExpressaoResidual ExpressaoAritmetica2'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">| </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "*"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExpressaoResidual ExpressaoAritmentica2'</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1415,7 +1557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1456,6 +1598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1770,24 +1913,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947A1816-5409-4DDA-AB90-1A65F65B0ACC}">
-  <dimension ref="B3:P79"/>
+  <dimension ref="B3:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" customWidth="1"/>
+    <col min="6" max="6" width="43" customWidth="1"/>
+    <col min="7" max="7" width="43.85546875" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.85546875" customWidth="1"/>
     <col min="15" max="15" width="6.42578125" customWidth="1"/>
@@ -1801,7 +1945,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1824,7 +1968,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -1841,13 +1985,13 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>20</v>
@@ -1872,7 +2016,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1889,7 +2033,7 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>2</v>
@@ -1920,7 +2064,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1937,13 +2081,13 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>20</v>
@@ -1967,7 +2111,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -1990,7 +2134,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -2007,13 +2151,13 @@
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
@@ -2061,7 +2205,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -2078,13 +2222,13 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>20</v>
@@ -2109,7 +2253,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6" t="s">
@@ -2163,7 +2307,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -2180,13 +2324,13 @@
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>20</v>
@@ -2248,7 +2392,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -2265,13 +2409,13 @@
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6" t="s">
@@ -2296,7 +2440,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -2319,7 +2463,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -2342,7 +2486,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -2365,7 +2509,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -2388,12 +2532,12 @@
         <v>2</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
@@ -2411,7 +2555,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="12"/>
@@ -2456,27 +2600,14 @@
       <c r="C30" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>134</v>
-      </c>
+      <c r="D30" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
@@ -2485,18 +2616,20 @@
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="6"/>
+        <v>125</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -2510,22 +2643,14 @@
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
+      <c r="D32" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
@@ -2535,22 +2660,32 @@
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
+      <c r="D33" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
@@ -2560,23 +2695,14 @@
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
+      <c r="D34" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
@@ -2585,23 +2711,20 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>53</v>
+      <c r="D35" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
+        <v>32</v>
+      </c>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
@@ -2610,20 +2733,17 @@
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>100</v>
-      </c>
+      <c r="D36" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
@@ -2633,54 +2753,58 @@
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>47</v>
+      <c r="D37" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>143</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>102</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
+        <v>116</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J38" t="s">
+        <v>119</v>
+      </c>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
@@ -2690,15 +2814,17 @@
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E39" s="6"/>
+      <c r="D39" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -2712,10 +2838,18 @@
       <c r="P39" s="6"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="B40" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -2729,138 +2863,188 @@
       <c r="P40" s="6"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="B41" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
-        <v>90</v>
-      </c>
+      <c r="B42" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
-        <v>7</v>
+      <c r="B44" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>4</v>
+      <c r="B61" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="2" t="s">
-        <v>78</v>
+      <c r="B62" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="2" t="s">
-        <v>6</v>
+      <c r="B63" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
@@ -2870,52 +3054,52 @@
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3" t="s">
-        <v>71</v>
+      <c r="B71" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
-        <v>68</v>
+      <c r="B77" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
@@ -2923,9 +3107,24 @@
         <v>66</v>
       </c>
     </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="B42:B79">
-    <sortCondition ref="B79"/>
+  <sortState ref="B45:B82">
+    <sortCondition ref="B82"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="D4:H4"/>

</xml_diff>